<commit_message>
Changed Excel and property file Location, New Classes
</commit_message>
<xml_diff>
--- a/FBAutomation/Data/CampaignData.xlsx
+++ b/FBAutomation/Data/CampaignData.xlsx
@@ -3,13 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SeleniumWorkspace\ws1\FBAutomation\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="5925" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Credentials" sheetId="2" r:id="rId1"/>
@@ -18,7 +13,8 @@
     <sheet name="CampaignAcquisition" sheetId="4" r:id="rId4"/>
     <sheet name="CamapignTrigger" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:B16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,9 +65,6 @@
     <t>SMS Acquisition 26 May</t>
   </si>
   <si>
-    <t>CampaignSMSBrod19may</t>
-  </si>
-  <si>
     <t>3OTaCGoiPP</t>
   </si>
   <si>
@@ -82,6 +75,9 @@
   </si>
   <si>
     <t>SMSBroadcast1June</t>
+  </si>
+  <si>
+    <t>CampaignSMSTrig19may</t>
   </si>
 </sst>
 </file>
@@ -472,9 +468,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -489,13 +485,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -513,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -527,7 +523,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -641,9 +637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -655,7 +649,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>6</v>

</xml_diff>